<commit_message>
Updated the examples - CSV and ODS files available
</commit_message>
<xml_diff>
--- a/Examples/XLSX/iris_virginica.xlsx
+++ b/Examples/XLSX/iris_virginica.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alkadri/Documents/These/Works/Current models/R_packages/databinders/Examples/XLSX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F84141C7-5B09-B54D-9ED2-BB7D8479ACB3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E32704-6F0A-A44D-9676-A14E87AC1DDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1460" windowWidth="27060" windowHeight="16040" xr2:uid="{F8E20B38-6311-7C47-8049-BF67CC032226}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E51"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>